<commit_message>
1. Added static methods wherever required
</commit_message>
<xml_diff>
--- a/dist/artifacts/log_c_structures.xlsx
+++ b/dist/artifacts/log_c_structures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D463D1DF-319C-4D8E-AF59-A5A79F4C80F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E18330-5C41-49E1-B6FD-EC6590F63C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{BA9F0090-5AAB-4A86-8EEE-D2B3967D6D75}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BA9F0090-5AAB-4A86-8EEE-D2B3967D6D75}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="9" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="149">
   <si>
     <t>field</t>
   </si>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t>bytes</t>
+  </si>
+  <si>
+    <t>MSG_MAINPUMP_GET_DRIVE_STAGE</t>
   </si>
 </sst>
 </file>
@@ -1466,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2004E192-DBD9-4258-A91C-5140AD1AFFA7}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1550,6 +1553,9 @@
       </c>
       <c r="F4">
         <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1919,7 +1925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845C0116-1AB4-4C77-9082-8AA73FAD2D5B}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1. added post status
</commit_message>
<xml_diff>
--- a/dist/artifacts/log_c_structures.xlsx
+++ b/dist/artifacts/log_c_structures.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E18330-5C41-49E1-B6FD-EC6590F63C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5726EC5-9F94-46E9-BBBF-704D91D5785F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BA9F0090-5AAB-4A86-8EEE-D2B3967D6D75}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{BA9F0090-5AAB-4A86-8EEE-D2B3967D6D75}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="9" r:id="rId1"/>
-    <sheet name="heater_cfg" sheetId="2" r:id="rId2"/>
-    <sheet name="bms_cfg" sheetId="1" r:id="rId3"/>
-    <sheet name="mainpump_cfg" sheetId="3" r:id="rId4"/>
-    <sheet name="valve_cfg" sheetId="4" r:id="rId5"/>
-    <sheet name="sensors_cfg" sheetId="6" r:id="rId6"/>
-    <sheet name="pressure_cfg" sheetId="8" r:id="rId7"/>
+    <sheet name="ccpd_post_st" sheetId="12" r:id="rId2"/>
+    <sheet name="uc_running_cfg" sheetId="11" r:id="rId3"/>
+    <sheet name="heater_cfg" sheetId="2" r:id="rId4"/>
+    <sheet name="bms_cfg" sheetId="1" r:id="rId5"/>
+    <sheet name="mainpump_cfg" sheetId="3" r:id="rId6"/>
+    <sheet name="valve_cfg" sheetId="4" r:id="rId7"/>
+    <sheet name="sensors_cfg" sheetId="6" r:id="rId8"/>
+    <sheet name="pressure_cfg" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="192">
   <si>
     <t>field</t>
   </si>
@@ -485,6 +487,135 @@
   </si>
   <si>
     <t>MSG_MAINPUMP_GET_DRIVE_STAGE</t>
+  </si>
+  <si>
+    <t>utilities/uc_helper.h</t>
+  </si>
+  <si>
+    <t>UC_RUNNING_CFG_STRUCT</t>
+  </si>
+  <si>
+    <t>uc_type</t>
+  </si>
+  <si>
+    <t>uc_state_id</t>
+  </si>
+  <si>
+    <t>uc_state_action</t>
+  </si>
+  <si>
+    <t>int8_t</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_RUN_UC_TYPE</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_RUN_UC_STATE_ID</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_RUN_UC_STATE_ACTION</t>
+  </si>
+  <si>
+    <t>usecase/uc_ccpd.c</t>
+  </si>
+  <si>
+    <t>begin_time_ms</t>
+  </si>
+  <si>
+    <t>mainpump_st</t>
+  </si>
+  <si>
+    <t>battery_st</t>
+  </si>
+  <si>
+    <t>ht_inlet_st</t>
+  </si>
+  <si>
+    <t>ht_outlet_st</t>
+  </si>
+  <si>
+    <t>ht_hpad1_st</t>
+  </si>
+  <si>
+    <t>ht_hpad2_st</t>
+  </si>
+  <si>
+    <t>heater_func_st</t>
+  </si>
+  <si>
+    <t>turb_top_st</t>
+  </si>
+  <si>
+    <t>turb_side_st</t>
+  </si>
+  <si>
+    <t>level_st</t>
+  </si>
+  <si>
+    <t>perit_st</t>
+  </si>
+  <si>
+    <t>airpressure_st</t>
+  </si>
+  <si>
+    <t>eeprom_st</t>
+  </si>
+  <si>
+    <t>fan_st</t>
+  </si>
+  <si>
+    <t>end_time_ms</t>
+  </si>
+  <si>
+    <t>CCPD_POST_ST_STRUCT</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_BEGIN_MS</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_MAINPUMP</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_BATTERY</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_HT_INLET</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_HT_OUTLET</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_HT_HPAD1</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_HT_HPAD2</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_HEATER_HEAT</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_TURB_TOP</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_TURB_SIDE</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_PERIT</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_LEVEL</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_AIRPA</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_EEPROM</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_FAN</t>
+  </si>
+  <si>
+    <t>MSG_UC_MASTER_GET_CCPD_POST_END_MS</t>
   </si>
 </sst>
 </file>
@@ -880,6 +1011,386 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4D38C8-1B17-4400-866A-4DA38F4C298E}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2">
+        <v>110</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>173</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A54FD6-4F65-4F7C-974F-AC4C3E72DD3F}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C571EA-EACA-4AD1-A4F5-C0841C8F776E}">
   <dimension ref="A1:G17"/>
   <sheetViews>
@@ -1145,7 +1656,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D7EC6D-77FA-479B-8461-A249A72FCD67}">
   <dimension ref="A1:G20"/>
   <sheetViews>
@@ -1465,11 +1976,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2004E192-DBD9-4258-A91C-5140AD1AFFA7}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="V1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1564,7 +2075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25A1163-282B-469D-BBC9-0BF22EA3DFB2}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1649,7 +2160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C44D35-35CF-4D00-8A9B-6BC1C9DC35FC}">
   <dimension ref="A1:G17"/>
   <sheetViews>
@@ -1921,7 +2432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845C0116-1AB4-4C77-9082-8AA73FAD2D5B}">
   <dimension ref="A1:G10"/>
   <sheetViews>

</xml_diff>

<commit_message>
1. added msg 2. cfg fix
</commit_message>
<xml_diff>
--- a/dist/artifacts/log_c_structures.xlsx
+++ b/dist/artifacts/log_c_structures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5726EC5-9F94-46E9-BBBF-704D91D5785F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7884BB-43A5-4350-9A53-EF37F052B9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{BA9F0090-5AAB-4A86-8EEE-D2B3967D6D75}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{BA9F0090-5AAB-4A86-8EEE-D2B3967D6D75}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="9" r:id="rId1"/>
@@ -1014,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4D38C8-1B17-4400-866A-4DA38F4C298E}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,7 +1080,7 @@
         <v>160</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1276,7 +1276,7 @@
         <v>174</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -1394,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C571EA-EACA-4AD1-A4F5-C0841C8F776E}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1605,7 +1605,7 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1619,7 +1619,7 @@
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1633,7 +1633,7 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1. added msg send panel
</commit_message>
<xml_diff>
--- a/dist/artifacts/log_c_structures.xlsx
+++ b/dist/artifacts/log_c_structures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7884BB-43A5-4350-9A53-EF37F052B9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB986977-C063-43C6-977A-DF0DC4A7267A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{BA9F0090-5AAB-4A86-8EEE-D2B3967D6D75}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{BA9F0090-5AAB-4A86-8EEE-D2B3967D6D75}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="196">
   <si>
     <t>field</t>
   </si>
@@ -616,6 +616,18 @@
   </si>
   <si>
     <t>MSG_UC_MASTER_GET_CCPD_POST_END_MS</t>
+  </si>
+  <si>
+    <t>MSG_BMS_GET_RUNNING_IN_BAT</t>
+  </si>
+  <si>
+    <t>is_running_in_bat</t>
+  </si>
+  <si>
+    <t>MSG_MAINPUMP_GET_STROKES_COUNT</t>
+  </si>
+  <si>
+    <t>strokes_count</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1027,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,7 +1092,7 @@
         <v>160</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1276,7 +1288,7 @@
         <v>174</v>
       </c>
       <c r="E17" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -1296,7 +1308,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1394,7 +1406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C571EA-EACA-4AD1-A4F5-C0841C8F776E}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1658,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D7EC6D-77FA-479B-8461-A249A72FCD67}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1709,74 +1721,77 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>28</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -1785,40 +1800,40 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -1827,12 +1842,12 @@
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -1841,12 +1856,12 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -1855,12 +1870,12 @@
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -1869,12 +1884,12 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
@@ -1883,26 +1898,23 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F15">
-        <v>4</v>
-      </c>
-      <c r="G15" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>17</v>
@@ -1911,12 +1923,12 @@
         <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
         <v>17</v>
@@ -1925,12 +1937,12 @@
         <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
         <v>17</v>
@@ -1939,35 +1951,49 @@
         <v>4</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G20" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1978,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2004E192-DBD9-4258-A91C-5140AD1AFFA7}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2029,21 +2055,21 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -2052,21 +2078,35 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>148</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. removed unused imports
</commit_message>
<xml_diff>
--- a/dist/artifacts/log_c_structures.xlsx
+++ b/dist/artifacts/log_c_structures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\apdcare\therapy_src\scripts\code_gen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AWAK_APD_CARE\raven-debug-framework\dist\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB986977-C063-43C6-977A-DF0DC4A7267A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BB092F-1456-4061-BC45-91AC770F3675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{BA9F0090-5AAB-4A86-8EEE-D2B3967D6D75}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA9F0090-5AAB-4A86-8EEE-D2B3967D6D75}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="9" r:id="rId1"/>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7510A3BC-D581-4EAC-B15C-256552C551A7}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,7 +1027,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,7 +1072,7 @@
         <v>175</v>
       </c>
       <c r="C2">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
         <v>159</v>
@@ -1308,7 +1308,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1353,7 +1353,7 @@
         <v>150</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>151</v>
@@ -1407,7 +1407,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1452,7 +1452,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -1673,7 +1673,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1718,7 +1718,7 @@
         <v>47</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -2006,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2004E192-DBD9-4258-A91C-5140AD1AFFA7}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2052,7 +2052,7 @@
         <v>49</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
@@ -2120,7 +2120,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2165,7 +2165,7 @@
         <v>54</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -2205,7 +2205,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2250,7 +2250,7 @@
         <v>92</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -2477,7 +2477,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2522,7 +2522,7 @@
         <v>124</v>
       </c>
       <c r="C2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>

</xml_diff>